<commit_message>
Added more test cases and logged more bugs.
</commit_message>
<xml_diff>
--- a/QA-Fund/Test-Management-and-Bug-Tracker-Template.xlsx
+++ b/QA-Fund/Test-Management-and-Bug-Tracker-Template.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Use Case 1" sheetId="1" state="visible" r:id="rId2"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="332" uniqueCount="201">
   <si>
     <t xml:space="preserve">Use Case 1: Landing Page</t>
   </si>
@@ -58,7 +58,7 @@
     <t xml:space="preserve">User is not logged in</t>
   </si>
   <si>
-    <t xml:space="preserve">Verify the Landing Page for not logged in users.</t>
+    <t xml:space="preserve">Verify The Landing Page</t>
   </si>
   <si>
     <t xml:space="preserve">1. Open the application.
@@ -76,7 +76,7 @@
     <t xml:space="preserve">Fail</t>
   </si>
   <si>
-    <t xml:space="preserve">Logged BUGID1</t>
+    <t xml:space="preserve">Logged BUG ID1</t>
   </si>
   <si>
     <t xml:space="preserve">UC1.2</t>
@@ -85,11 +85,11 @@
     <t xml:space="preserve">User is not logged in </t>
   </si>
   <si>
-    <t xml:space="preserve">Verify the “Optimize Your Time Now!” button. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.Open the application
-2.Click “Optimize Your Time Now!” button</t>
+    <t xml:space="preserve">Verify “Optimize  Your Time Now!” button </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.Open the application 
+2.Click on “Optimize  Your Time Now!” button </t>
   </si>
   <si>
     <t xml:space="preserve">User is navigated  to the Register form</t>
@@ -126,7 +126,7 @@
     <t xml:space="preserve">User is navigated to the Terms of Service page </t>
   </si>
   <si>
-    <t xml:space="preserve">Logged BUGID2</t>
+    <t xml:space="preserve">Logged BUG ID2</t>
   </si>
   <si>
     <t xml:space="preserve">* If you want to add a new line in a cell, use Alt + Enter</t>
@@ -267,7 +267,7 @@
     <t xml:space="preserve">User is not able to enter more symbols than specified ones.</t>
   </si>
   <si>
-    <t xml:space="preserve">Logged BUGID4</t>
+    <t xml:space="preserve">Logged BUG ID4</t>
   </si>
   <si>
     <t xml:space="preserve">UC2.7</t>
@@ -307,7 +307,7 @@
     <t xml:space="preserve">Successful Login </t>
   </si>
   <si>
-    <t xml:space="preserve">Logged BUGID5</t>
+    <t xml:space="preserve">Logged BUG ID5</t>
   </si>
   <si>
     <t xml:space="preserve">Priority options:</t>
@@ -330,7 +330,7 @@
     <t xml:space="preserve">Validation massage should appear </t>
   </si>
   <si>
-    <t xml:space="preserve">Logged BUGID6</t>
+    <t xml:space="preserve">Logged BUG ID6</t>
   </si>
   <si>
     <t xml:space="preserve">UC3.3</t>
@@ -347,7 +347,7 @@
     <t xml:space="preserve">User should be redirected to the “Restore Password” page </t>
   </si>
   <si>
-    <t xml:space="preserve">Logged BUGID7</t>
+    <t xml:space="preserve">Logged BUG ID7</t>
   </si>
   <si>
     <t xml:space="preserve">2. High</t>
@@ -373,6 +373,7 @@
         <sz val="11"/>
         <rFont val="Calibri"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">1</t>
     </r>
@@ -382,6 +383,7 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">.Open the application
  2. Log in with “Bob”</t>
@@ -409,6 +411,7 @@
         <sz val="11"/>
         <rFont val="Calibri"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">-Navigation bar</t>
     </r>
@@ -418,6 +421,7 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> 
 -Home Page link on the left
@@ -446,6 +450,7 @@
         <sz val="11"/>
         <rFont val="Calibri"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">1.Login with “Bob</t>
     </r>
@@ -455,6 +460,7 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">”
 2.Click on Profile icon </t>
@@ -466,6 +472,7 @@
         <sz val="11"/>
         <rFont val="Calibri"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Verify the following sections are displayed:</t>
     </r>
@@ -475,6 +482,7 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> 
 -User avatar picture 
@@ -488,7 +496,7 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">Logged BUGID8</t>
+    <t xml:space="preserve">Logged BUG ID8</t>
   </si>
   <si>
     <t xml:space="preserve">UC5.2</t>
@@ -502,8 +510,10 @@
         <sz val="11"/>
         <rFont val="Calibri"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">1.Login with “Bob”</t>
+      <t xml:space="preserve">
+</t>
     </r>
     <r>
       <rPr>
@@ -511,10 +521,10 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
-      <t xml:space="preserve"> 
-2.Click on Profile icon 
-3.Click “EDIT PROFILE INFO” button </t>
+      <t xml:space="preserve">1.Click on Profile icon 
+2.Click “EDIT PROFILE INFO” button </t>
     </r>
   </si>
   <si>
@@ -523,6 +533,7 @@
         <sz val="11"/>
         <rFont val="Calibri"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Verify the following fields are displayed:</t>
     </r>
@@ -532,6 +543,7 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> 
 -First Name 
@@ -542,7 +554,7 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">Logged BUGID9</t>
+    <t xml:space="preserve">Logged BUG ID9</t>
   </si>
   <si>
     <t xml:space="preserve">UC5.3</t>
@@ -559,6 +571,7 @@
         <sz val="11"/>
         <rFont val="Calibri"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">1.Navigate to Avatar Picture field</t>
     </r>
@@ -568,6 +581,7 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> 
 2. input a valid url (http://......jpg)
@@ -578,22 +592,7 @@
     <t xml:space="preserve">The user’s profile picture should change to the picture provided by the url</t>
   </si>
   <si>
-    <t xml:space="preserve">'</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Use Case 6: Task Creation and Management</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Description</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UC6.1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">User “Bob” is logged in </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Verify all required fields </t>
+    <t xml:space="preserve">UC5.4</t>
   </si>
   <si>
     <r>
@@ -601,6 +600,101 @@
         <sz val="11"/>
         <rFont val="Calibri"/>
         <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">'</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">User “Bob” is logged in and is editing his profile</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify Social Media links </t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">1.Click on Profile icon 
+2.Click on the Social Media buttons </t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Login Form will open depending on the clicked link</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Logged BUG ID13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UC5.5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify “EDIT PROFILE INFO” button </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.Click on Profile icon 
+2.Click on “EDIT PROFILE INFO” button</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The “Edit Profile Info Page” should open </t>
+  </si>
+  <si>
+    <t xml:space="preserve">UC5.6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify that you can edit your profile info</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.Click on Profile icon 
+2.Click on “Edit” button</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Users should be able to update their First Name, Middle Name, Last Name and Avatar Picture </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Logged BUG ID12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Use Case 6: Task Creation and Management</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Description</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UC6.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">User “Bob” is logged in </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify all required validation messages when creating a task</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">1.Navigate to Task creation page
 </t>
@@ -611,21 +705,22 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">2.Click on “Create” </t>
     </r>
   </si>
   <si>
-    <t xml:space="preserve">All validation massages should be displayed </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Logged BUGID10</t>
+    <t xml:space="preserve">All validation messages should be displayed </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Logged BUG ID10</t>
   </si>
   <si>
     <t xml:space="preserve">UC6.2</t>
   </si>
   <si>
-    <t xml:space="preserve">Verify required labels</t>
+    <t xml:space="preserve">Verify required fields and labels</t>
   </si>
   <si>
     <t xml:space="preserve">1.Navigate to Task creation page</t>
@@ -636,6 +731,7 @@
         <sz val="11"/>
         <rFont val="Calibri"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Create New Task form is opened with the following fields:
 </t>
@@ -646,6 +742,7 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">-TaskName
 -Description
@@ -656,6 +753,9 @@
     </r>
   </si>
   <si>
+    <t xml:space="preserve">UC6.3</t>
+  </si>
+  <si>
     <t xml:space="preserve">User “Bob” is logged in and a task exists </t>
   </si>
   <si>
@@ -667,6 +767,7 @@
         <sz val="11"/>
         <rFont val="Calibri"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">1.Navigate to Task
 </t>
@@ -677,6 +778,7 @@
         <color rgb="FF000000"/>
         <rFont val="Calibri"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">2.Click on “EDIT” button
 3.Click on “DELETE” button</t>
@@ -684,6 +786,23 @@
   </si>
   <si>
     <t xml:space="preserve">buttons enable the user to modify the task's details or remove the task from the board entirely.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UC6.4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify validation message when deleting a task</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.Navigate to Task Navbar 
+2.Navigate to Task 
+3.Click “DELETE”</t>
+  </si>
+  <si>
+    <t xml:space="preserve">a validation message should appear asking if you are sure about deleting this task </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Logged BUG ID11</t>
   </si>
   <si>
     <t xml:space="preserve">Bug Report</t>
@@ -754,7 +873,7 @@
  - Middle Name;
  - Last name;
  - Password;
- - Repaeat Password;
+ - Repeat Password;
  - Terms and conditions hyperlink </t>
   </si>
   <si>
@@ -765,7 +884,7 @@
  - Middle Name;
  - Middle Name;
  - Password;
- - Repaeat Password;
+ - Repeat Password;
  - Terms and conditions hyperlink </t>
   </si>
   <si>
@@ -801,7 +920,7 @@
     <t xml:space="preserve">No validation massage </t>
   </si>
   <si>
-    <t xml:space="preserve">Critical</t>
+    <t xml:space="preserve">Blocking</t>
   </si>
   <si>
     <t xml:space="preserve">Forgot Password link does not work</t>
@@ -831,6 +950,9 @@
     <t xml:space="preserve">Missing First name and Last name fields</t>
   </si>
   <si>
+    <t xml:space="preserve">Critical</t>
+  </si>
+  <si>
     <t xml:space="preserve">“EDIT PROFILE INFO” button does not work</t>
   </si>
   <si>
@@ -844,13 +966,13 @@
 -Middle Name
 -Last Name 
 -Avatar Picture 
-“Edit” button and “Cancel” button displayed</t>
+“Edit” button and “Cancel” button displayed and working </t>
   </si>
   <si>
     <t xml:space="preserve">“EDIT PROFILE INFO” button does not work.</t>
   </si>
   <si>
-    <t xml:space="preserve">Spelling mistake in validation massage </t>
+    <t xml:space="preserve">Spelling mistake in validation message </t>
   </si>
   <si>
     <t xml:space="preserve">1.Navigate to Task Creation Page and enter all fields except Status</t>
@@ -860,6 +982,28 @@
   </si>
   <si>
     <t xml:space="preserve">“Please choice a task!” massage is displayed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Spelling mistake in validation message</t>
+  </si>
+  <si>
+    <t xml:space="preserve">a validation message should appear asking if you are sure about deleting this task “Are you sure you want to delete this task?”</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Instead its “Are you sure you want to delte this task?” spellin mistake “delte”</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Users cannot edit Profile info </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Upon entering the “Edit Profile Info” page clicking on “Edit” button after making changes does not save those changes </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Social Media links don’t work</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.Click on Profile icon 
+2.Click on the Social Media buttons </t>
   </si>
 </sst>
 </file>
@@ -869,12 +1013,13 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="35">
+  <fonts count="37">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -892,29 +1037,34 @@
       <family val="0"/>
     </font>
     <font>
+      <sz val="10"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Arial"/>
+      <family val="0"/>
+      <charset val="1"/>
+    </font>
+    <font>
       <b val="true"/>
-      <sz val="24"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="0"/>
-    </font>
-    <font>
-      <sz val="18"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
-      <color rgb="FF333333"/>
+      <color rgb="FFCC0000"/>
       <name val="Arial"/>
       <family val="0"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Arial"/>
+      <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
       <i val="true"/>
@@ -922,6 +1072,36 @@
       <color rgb="FF808080"/>
       <name val="Arial"/>
       <family val="0"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF006600"/>
+      <name val="Arial"/>
+      <family val="0"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="0"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="0"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="24"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
       <u val="single"/>
@@ -929,50 +1109,28 @@
       <color rgb="FF0000EE"/>
       <name val="Arial"/>
       <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF006600"/>
-      <name val="Arial"/>
-      <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF996600"/>
       <name val="Arial"/>
       <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
-      <color rgb="FFCC0000"/>
+      <color rgb="FF333333"/>
       <name val="Arial"/>
       <family val="0"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="10"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Arial"/>
-      <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -980,6 +1138,7 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -987,17 +1146,20 @@
       <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
       <sz val="12"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -1005,6 +1167,7 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -1012,6 +1175,14 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
@@ -1023,6 +1194,7 @@
       <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -1030,37 +1202,49 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
       <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -1070,18 +1254,21 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="13">
@@ -1090,30 +1277,6 @@
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor rgb="FFFFFFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFCCFFCC"/>
-        <bgColor rgb="FFCCFFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCCCC"/>
-        <bgColor rgb="FFDDDDDD"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFCC0000"/>
-        <bgColor rgb="FFFF0000"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -1131,6 +1294,30 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFDDDDDD"/>
         <bgColor rgb="FFFFCCCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCCCC"/>
+        <bgColor rgb="FFDDDDDD"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCC0000"/>
+        <bgColor rgb="FFFF0000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCCFFCC"/>
+        <bgColor rgb="FFCCFFFF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor rgb="FFFFFFFF"/>
       </patternFill>
     </fill>
     <fill>
@@ -1256,66 +1443,66 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="4" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="5" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="6" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="7" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="8" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="8" borderId="1" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="2" borderId="1" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="3" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="2" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="4" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="13" fillId="5" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="15" fillId="6" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="15" fillId="7" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="14" fillId="8" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="18" fillId="9" borderId="2" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="58">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1360,6 +1547,10 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="24" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="23" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1368,7 +1559,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="24" fillId="11" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="25" fillId="11" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1384,14 +1575,14 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="20" fillId="10" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1404,11 +1595,11 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="27" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="28" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="24" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="25" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1424,14 +1615,14 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="20" fillId="10" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1444,43 +1635,55 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="27" fillId="0" borderId="3" xfId="37" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="32" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="28" fillId="0" borderId="3" xfId="35" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="24" fillId="0" borderId="3" xfId="37" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="25" fillId="0" borderId="3" xfId="35" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="37" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="35" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="26" fillId="0" borderId="0" xfId="37" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="27" fillId="0" borderId="0" xfId="35" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="23" fillId="0" borderId="3" xfId="37" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="23" fillId="0" borderId="3" xfId="35" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="33" fillId="0" borderId="3" xfId="35" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="24" fillId="0" borderId="3" xfId="35" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="33" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="32" fillId="12" borderId="3" xfId="38" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="34" fillId="12" borderId="3" xfId="38" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1500,7 +1703,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="33" fillId="12" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="35" fillId="12" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1516,15 +1719,15 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="27" fillId="0" borderId="3" xfId="37" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="28" fillId="0" borderId="3" xfId="35" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="27" fillId="11" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="28" fillId="11" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="34" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="36" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1540,24 +1743,24 @@
     <cellStyle name="Currency" xfId="17" builtinId="4"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
-    <cellStyle name="Heading" xfId="20"/>
-    <cellStyle name="Heading 1" xfId="21"/>
-    <cellStyle name="Heading 2" xfId="22"/>
-    <cellStyle name="Text" xfId="23"/>
-    <cellStyle name="Note" xfId="24"/>
-    <cellStyle name="Footnote" xfId="25"/>
-    <cellStyle name="Hyperlink" xfId="26"/>
-    <cellStyle name="Status" xfId="27"/>
-    <cellStyle name="Good" xfId="28"/>
-    <cellStyle name="Neutral" xfId="29"/>
-    <cellStyle name="Bad" xfId="30"/>
-    <cellStyle name="Warning" xfId="31"/>
-    <cellStyle name="Error" xfId="32"/>
-    <cellStyle name="Accent" xfId="33"/>
-    <cellStyle name="Accent 1" xfId="34"/>
-    <cellStyle name="Accent 2" xfId="35"/>
-    <cellStyle name="Accent 3" xfId="36"/>
-    <cellStyle name="Style 1" xfId="37"/>
+    <cellStyle name="Accent 1 17" xfId="20"/>
+    <cellStyle name="Accent 16" xfId="21"/>
+    <cellStyle name="Accent 2 18" xfId="22"/>
+    <cellStyle name="Accent 3 19" xfId="23"/>
+    <cellStyle name="Bad 13" xfId="24"/>
+    <cellStyle name="Error 15" xfId="25"/>
+    <cellStyle name="Footnote 8" xfId="26"/>
+    <cellStyle name="Good 11" xfId="27"/>
+    <cellStyle name="Heading 1 4" xfId="28"/>
+    <cellStyle name="Heading 2 5" xfId="29"/>
+    <cellStyle name="Heading 3" xfId="30"/>
+    <cellStyle name="Hyperlink 9" xfId="31"/>
+    <cellStyle name="Neutral 12" xfId="32"/>
+    <cellStyle name="Note 7" xfId="33"/>
+    <cellStyle name="Status 10" xfId="34"/>
+    <cellStyle name="Style 1" xfId="35"/>
+    <cellStyle name="Text 6" xfId="36"/>
+    <cellStyle name="Warning 14" xfId="37"/>
     <cellStyle name="Excel Built-in Check Cell" xfId="38"/>
   </cellStyles>
   <colors>
@@ -1714,22 +1917,22 @@
   </sheetPr>
   <dimension ref="A1:P14"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="D4" activeCellId="0" sqref="D4"/>
+      <selection pane="bottomLeft" activeCell="D6" activeCellId="0" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="10.77"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="15.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="15.79"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="45.77"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="50.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="50.79"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="40.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="12.22"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="40.78"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="8" style="1" width="14.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="8" style="1" width="14.43"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1778,52 +1981,52 @@
       </c>
       <c r="P3" s="8"/>
     </row>
-    <row r="4" s="12" customFormat="true" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" s="13" customFormat="true" ht="91.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="9" t="s">
         <v>8</v>
       </c>
       <c r="B4" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="10" t="s">
+      <c r="C4" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="10" t="s">
+      <c r="D4" s="11" t="s">
         <v>11</v>
       </c>
       <c r="E4" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="F4" s="11" t="s">
+      <c r="F4" s="12" t="s">
         <v>13</v>
       </c>
       <c r="G4" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="P4" s="13"/>
-    </row>
-    <row r="5" s="12" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="P4" s="14"/>
+    </row>
+    <row r="5" s="13" customFormat="true" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="9" t="s">
         <v>15</v>
       </c>
       <c r="B5" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="C5" s="10" t="s">
+      <c r="C5" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="D5" s="10" t="s">
+      <c r="D5" s="11" t="s">
         <v>18</v>
       </c>
       <c r="E5" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="F5" s="11" t="s">
+      <c r="F5" s="12" t="s">
         <v>20</v>
       </c>
       <c r="G5" s="10"/>
     </row>
-    <row r="6" s="14" customFormat="true" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" s="15" customFormat="true" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="9" t="s">
         <v>21</v>
       </c>
@@ -1844,7 +2047,7 @@
       </c>
       <c r="G6" s="10"/>
     </row>
-    <row r="7" s="14" customFormat="true" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" s="15" customFormat="true" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="9" t="s">
         <v>25</v>
       </c>
@@ -1863,11 +2066,11 @@
       <c r="F7" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="G7" s="15" t="s">
+      <c r="G7" s="16" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="8" s="16" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" s="17" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="9"/>
       <c r="B8" s="10"/>
       <c r="C8" s="10"/>
@@ -1876,17 +2079,17 @@
       <c r="F8" s="10"/>
       <c r="G8" s="10"/>
     </row>
-    <row r="9" s="12" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" s="13" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="9"/>
       <c r="B9" s="10"/>
       <c r="C9" s="10"/>
       <c r="D9" s="10"/>
       <c r="E9" s="10"/>
       <c r="F9" s="10"/>
-      <c r="G9" s="15"/>
-      <c r="P9" s="13"/>
-    </row>
-    <row r="10" s="12" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G9" s="16"/>
+      <c r="P9" s="14"/>
+    </row>
+    <row r="10" s="13" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="9"/>
       <c r="B10" s="10"/>
       <c r="C10" s="10"/>
@@ -1895,17 +2098,17 @@
       <c r="F10" s="10"/>
       <c r="G10" s="10"/>
     </row>
-    <row r="11" s="14" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" s="15" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="9"/>
       <c r="B11" s="10"/>
       <c r="C11" s="10"/>
       <c r="D11" s="10"/>
       <c r="E11" s="10"/>
       <c r="F11" s="10"/>
-      <c r="G11" s="15"/>
+      <c r="G11" s="16"/>
     </row>
     <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="17" t="s">
+      <c r="A14" s="18" t="s">
         <v>30</v>
       </c>
     </row>
@@ -1940,21 +2143,21 @@
   <dimension ref="A1:P11"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="3" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="D9" activeCellId="0" sqref="D9"/>
+      <selection pane="bottomLeft" activeCell="G9" activeCellId="0" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.77"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.79"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="45.77"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="50.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="50.79"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="45.77"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="10.77"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="40.78"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="8" style="0" width="14.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="8" style="0" width="14.43"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1967,7 +2170,7 @@
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
       <c r="G1" s="2"/>
-      <c r="P1" s="18"/>
+      <c r="P1" s="19"/>
     </row>
     <row r="2" customFormat="false" ht="15.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="2"/>
@@ -1977,37 +2180,37 @@
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
-      <c r="P2" s="18"/>
+      <c r="P2" s="19"/>
     </row>
     <row r="3" customFormat="false" ht="28.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="19" t="s">
+      <c r="A3" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="19" t="s">
+      <c r="B3" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="20" t="s">
+      <c r="C3" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="19" t="s">
+      <c r="D3" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="19" t="s">
+      <c r="E3" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="21" t="s">
+      <c r="F3" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="G3" s="21" t="s">
+      <c r="G3" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="P3" s="18"/>
+      <c r="P3" s="19"/>
     </row>
     <row r="4" customFormat="false" ht="102.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="22" t="s">
+      <c r="A4" s="23" t="s">
         <v>32</v>
       </c>
-      <c r="B4" s="23" t="s">
+      <c r="B4" s="24" t="s">
         <v>9</v>
       </c>
       <c r="C4" s="10" t="s">
@@ -2025,13 +2228,13 @@
       <c r="G4" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="P4" s="18"/>
+      <c r="P4" s="19"/>
     </row>
     <row r="5" customFormat="false" ht="102.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="22" t="s">
+      <c r="A5" s="23" t="s">
         <v>37</v>
       </c>
-      <c r="B5" s="23" t="s">
+      <c r="B5" s="24" t="s">
         <v>9</v>
       </c>
       <c r="C5" s="10" t="s">
@@ -2047,13 +2250,13 @@
         <v>20</v>
       </c>
       <c r="G5" s="10"/>
-      <c r="P5" s="18"/>
+      <c r="P5" s="19"/>
     </row>
     <row r="6" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="22" t="s">
+      <c r="A6" s="23" t="s">
         <v>41</v>
       </c>
-      <c r="B6" s="23" t="s">
+      <c r="B6" s="24" t="s">
         <v>9</v>
       </c>
       <c r="C6" s="10" t="s">
@@ -2069,13 +2272,13 @@
         <v>20</v>
       </c>
       <c r="G6" s="10"/>
-      <c r="P6" s="18"/>
+      <c r="P6" s="19"/>
     </row>
     <row r="7" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="22" t="s">
+      <c r="A7" s="23" t="s">
         <v>45</v>
       </c>
-      <c r="B7" s="23" t="s">
+      <c r="B7" s="24" t="s">
         <v>9</v>
       </c>
       <c r="C7" s="10" t="s">
@@ -2091,13 +2294,13 @@
         <v>20</v>
       </c>
       <c r="G7" s="10"/>
-      <c r="P7" s="18"/>
+      <c r="P7" s="19"/>
     </row>
     <row r="8" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="22" t="s">
+      <c r="A8" s="23" t="s">
         <v>49</v>
       </c>
-      <c r="B8" s="23" t="s">
+      <c r="B8" s="24" t="s">
         <v>16</v>
       </c>
       <c r="C8" s="10" t="s">
@@ -2115,13 +2318,13 @@
       <c r="G8" s="10"/>
     </row>
     <row r="9" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="22" t="s">
+      <c r="A9" s="23" t="s">
         <v>52</v>
       </c>
-      <c r="B9" s="23" t="s">
+      <c r="B9" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="C9" s="24" t="s">
+      <c r="C9" s="25" t="s">
         <v>53</v>
       </c>
       <c r="D9" s="10" t="s">
@@ -2138,13 +2341,13 @@
       </c>
     </row>
     <row r="10" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="22" t="s">
+      <c r="A10" s="23" t="s">
         <v>57</v>
       </c>
-      <c r="B10" s="23" t="s">
+      <c r="B10" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="C10" s="24" t="s">
+      <c r="C10" s="25" t="s">
         <v>58</v>
       </c>
       <c r="D10" s="10" t="s">
@@ -2159,9 +2362,9 @@
       <c r="G10" s="10"/>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="22"/>
-      <c r="B11" s="23"/>
-      <c r="C11" s="24"/>
+      <c r="A11" s="23"/>
+      <c r="B11" s="24"/>
+      <c r="C11" s="25"/>
       <c r="D11" s="10"/>
       <c r="E11" s="10"/>
       <c r="F11" s="10"/>
@@ -2200,19 +2403,19 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="E6" activeCellId="0" sqref="E6"/>
+      <selection pane="bottomLeft" activeCell="G4" activeCellId="0" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.77"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.79"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="45.77"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="50.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="50.79"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="45.77"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="11.77"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="40.78"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="8" style="0" width="14.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="8" style="0" width="14.43"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2225,7 +2428,7 @@
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
       <c r="G1" s="2"/>
-      <c r="P1" s="18"/>
+      <c r="P1" s="19"/>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="2"/>
@@ -2235,91 +2438,91 @@
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
-      <c r="P2" s="18"/>
+      <c r="P2" s="19"/>
     </row>
     <row r="3" customFormat="false" ht="28.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="19" t="s">
+      <c r="A3" s="20" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="20" t="s">
+      <c r="B3" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="19" t="s">
+      <c r="C3" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="19" t="s">
+      <c r="D3" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="19" t="s">
+      <c r="E3" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="21" t="s">
+      <c r="F3" s="22" t="s">
         <v>6</v>
       </c>
       <c r="G3" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="P3" s="18"/>
-    </row>
-    <row r="4" s="27" customFormat="true" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="25" t="s">
+      <c r="P3" s="19"/>
+    </row>
+    <row r="4" s="28" customFormat="true" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="26" t="s">
         <v>62</v>
       </c>
-      <c r="B4" s="26" t="s">
+      <c r="B4" s="27" t="s">
         <v>63</v>
       </c>
-      <c r="C4" s="26" t="s">
+      <c r="C4" s="27" t="s">
         <v>64</v>
       </c>
       <c r="D4" s="10" t="s">
         <v>65</v>
       </c>
-      <c r="E4" s="26" t="s">
+      <c r="E4" s="27" t="s">
         <v>66</v>
       </c>
-      <c r="F4" s="26" t="s">
+      <c r="F4" s="27" t="s">
         <v>13</v>
       </c>
-      <c r="G4" s="24" t="s">
+      <c r="G4" s="25" t="s">
         <v>67</v>
       </c>
-      <c r="O4" s="28" t="s">
+      <c r="O4" s="29" t="s">
         <v>68</v>
       </c>
-      <c r="P4" s="28" t="s">
+      <c r="P4" s="29" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="5" s="27" customFormat="true" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="25" t="s">
+    <row r="5" s="28" customFormat="true" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="26" t="s">
         <v>70</v>
       </c>
-      <c r="B5" s="26" t="s">
+      <c r="B5" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="26" t="s">
+      <c r="C5" s="27" t="s">
         <v>71</v>
       </c>
       <c r="D5" s="10" t="s">
         <v>72</v>
       </c>
-      <c r="E5" s="26" t="s">
+      <c r="E5" s="27" t="s">
         <v>73</v>
       </c>
-      <c r="F5" s="26" t="s">
+      <c r="F5" s="27" t="s">
         <v>13</v>
       </c>
       <c r="G5" s="10" t="s">
         <v>74</v>
       </c>
-      <c r="O5" s="28"/>
-      <c r="P5" s="28"/>
-    </row>
-    <row r="6" s="27" customFormat="true" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="25" t="s">
+      <c r="O5" s="29"/>
+      <c r="P5" s="29"/>
+    </row>
+    <row r="6" s="28" customFormat="true" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="26" t="s">
         <v>75</v>
       </c>
-      <c r="B6" s="26" t="s">
+      <c r="B6" s="27" t="s">
         <v>16</v>
       </c>
       <c r="C6" s="10" t="s">
@@ -2331,57 +2534,57 @@
       <c r="E6" s="10" t="s">
         <v>78</v>
       </c>
-      <c r="F6" s="26" t="s">
+      <c r="F6" s="27" t="s">
         <v>13</v>
       </c>
       <c r="G6" s="10" t="s">
         <v>79</v>
       </c>
-      <c r="O6" s="28"/>
-      <c r="P6" s="28"/>
-    </row>
-    <row r="7" s="27" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="25"/>
-      <c r="B7" s="26"/>
+      <c r="O6" s="29"/>
+      <c r="P6" s="29"/>
+    </row>
+    <row r="7" s="28" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="26"/>
+      <c r="B7" s="27"/>
       <c r="C7" s="10"/>
       <c r="D7" s="10"/>
       <c r="E7" s="10"/>
       <c r="F7" s="10"/>
       <c r="G7" s="10"/>
-      <c r="O7" s="28"/>
-      <c r="P7" s="28"/>
-    </row>
-    <row r="8" s="27" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="25"/>
-      <c r="B8" s="26"/>
-      <c r="C8" s="26"/>
+      <c r="O7" s="29"/>
+      <c r="P7" s="29"/>
+    </row>
+    <row r="8" s="28" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="26"/>
+      <c r="B8" s="27"/>
+      <c r="C8" s="27"/>
       <c r="D8" s="10"/>
       <c r="E8" s="10"/>
-      <c r="F8" s="26"/>
+      <c r="F8" s="27"/>
       <c r="G8" s="10"/>
-      <c r="P8" s="28" t="s">
+      <c r="P8" s="29" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="9" s="27" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="25"/>
-      <c r="B9" s="26"/>
+    <row r="9" s="28" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="26"/>
+      <c r="B9" s="27"/>
       <c r="C9" s="10"/>
       <c r="D9" s="10"/>
       <c r="E9" s="10"/>
-      <c r="F9" s="26"/>
+      <c r="F9" s="27"/>
       <c r="G9" s="10"/>
-      <c r="P9" s="28" t="s">
+      <c r="P9" s="29" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="25"/>
-      <c r="B10" s="26"/>
+      <c r="A10" s="26"/>
+      <c r="B10" s="27"/>
       <c r="C10" s="10"/>
       <c r="D10" s="10"/>
       <c r="E10" s="10"/>
-      <c r="F10" s="26"/>
+      <c r="F10" s="27"/>
       <c r="G10" s="10"/>
     </row>
   </sheetData>
@@ -2389,11 +2592,11 @@
     <mergeCell ref="A1:G2"/>
   </mergeCells>
   <dataValidations count="2">
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="F4:F10" type="list">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="F1:F2" type="list">
       <formula1>"Pass,Fail"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="F1:F2" type="list">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="F4:F10" type="list">
       <formula1>"Pass,Fail"</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -2418,7 +2621,7 @@
   </sheetPr>
   <dimension ref="A1:P13"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="bottomLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
@@ -2427,13 +2630,13 @@
   <sheetFormatPr defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.77"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.79"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="45.77"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="50.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="50.79"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="45.77"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="11.77"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="40.78"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="8" style="0" width="14.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="8" style="0" width="14.43"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2446,7 +2649,7 @@
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
       <c r="G1" s="2"/>
-      <c r="P1" s="18"/>
+      <c r="P1" s="19"/>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="2"/>
@@ -2456,160 +2659,160 @@
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
-      <c r="P2" s="18"/>
-    </row>
-    <row r="3" s="32" customFormat="true" ht="28.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="29" t="s">
+      <c r="P2" s="19"/>
+    </row>
+    <row r="3" s="33" customFormat="true" ht="28.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="30" t="s">
+      <c r="B3" s="31" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="29" t="s">
+      <c r="C3" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="29" t="s">
+      <c r="D3" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="29" t="s">
+      <c r="E3" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="31" t="s">
+      <c r="F3" s="32" t="s">
         <v>6</v>
       </c>
-      <c r="G3" s="31" t="s">
+      <c r="G3" s="32" t="s">
         <v>7</v>
       </c>
-      <c r="P3" s="33"/>
-    </row>
-    <row r="4" s="36" customFormat="true" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="34" t="s">
+      <c r="P3" s="34"/>
+    </row>
+    <row r="4" s="37" customFormat="true" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="35" t="s">
         <v>83</v>
       </c>
-      <c r="B4" s="35" t="s">
+      <c r="B4" s="36" t="s">
         <v>84</v>
       </c>
       <c r="C4" s="10" t="s">
         <v>85</v>
       </c>
-      <c r="D4" s="35" t="s">
+      <c r="D4" s="36" t="s">
         <v>86</v>
       </c>
       <c r="E4" s="10" t="s">
         <v>87</v>
       </c>
-      <c r="F4" s="35" t="s">
+      <c r="F4" s="36" t="s">
         <v>20</v>
       </c>
-      <c r="G4" s="35"/>
-      <c r="O4" s="37" t="s">
+      <c r="G4" s="36"/>
+      <c r="O4" s="38" t="s">
         <v>68</v>
       </c>
-      <c r="P4" s="37" t="s">
+      <c r="P4" s="38" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="5" s="36" customFormat="true" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="34" t="s">
+    <row r="5" s="37" customFormat="true" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="35" t="s">
         <v>88</v>
       </c>
-      <c r="B5" s="35" t="s">
+      <c r="B5" s="36" t="s">
         <v>89</v>
       </c>
-      <c r="C5" s="35" t="s">
+      <c r="C5" s="36" t="s">
         <v>90</v>
       </c>
-      <c r="D5" s="38" t="s">
+      <c r="D5" s="39" t="s">
         <v>91</v>
       </c>
-      <c r="E5" s="35" t="s">
+      <c r="E5" s="36" t="s">
         <v>92</v>
       </c>
-      <c r="F5" s="35" t="s">
+      <c r="F5" s="36" t="s">
         <v>20</v>
       </c>
-      <c r="G5" s="35"/>
-      <c r="P5" s="37" t="s">
+      <c r="G5" s="36"/>
+      <c r="P5" s="38" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="6" s="36" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="34"/>
-      <c r="B6" s="35"/>
-      <c r="C6" s="35"/>
-      <c r="D6" s="35"/>
-      <c r="E6" s="35"/>
-      <c r="F6" s="35"/>
-      <c r="G6" s="35"/>
-      <c r="P6" s="37"/>
-    </row>
-    <row r="7" s="36" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="34"/>
-      <c r="B7" s="35"/>
-      <c r="C7" s="35"/>
-      <c r="D7" s="35"/>
-      <c r="E7" s="35"/>
-      <c r="F7" s="35"/>
-      <c r="G7" s="35"/>
-      <c r="P7" s="37"/>
-    </row>
-    <row r="8" s="36" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="34"/>
-      <c r="B8" s="35"/>
-      <c r="C8" s="35"/>
-      <c r="D8" s="35"/>
-      <c r="E8" s="35"/>
-      <c r="F8" s="35"/>
-      <c r="G8" s="35"/>
-      <c r="P8" s="37"/>
-    </row>
-    <row r="9" s="36" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="34"/>
-      <c r="B9" s="35"/>
-      <c r="C9" s="35"/>
-      <c r="D9" s="35"/>
-      <c r="E9" s="35"/>
-      <c r="F9" s="35"/>
-      <c r="G9" s="35"/>
-      <c r="P9" s="37" t="s">
+    <row r="6" s="37" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="35"/>
+      <c r="B6" s="36"/>
+      <c r="C6" s="36"/>
+      <c r="D6" s="36"/>
+      <c r="E6" s="36"/>
+      <c r="F6" s="36"/>
+      <c r="G6" s="36"/>
+      <c r="P6" s="38"/>
+    </row>
+    <row r="7" s="37" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="35"/>
+      <c r="B7" s="36"/>
+      <c r="C7" s="36"/>
+      <c r="D7" s="36"/>
+      <c r="E7" s="36"/>
+      <c r="F7" s="36"/>
+      <c r="G7" s="36"/>
+      <c r="P7" s="38"/>
+    </row>
+    <row r="8" s="37" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="35"/>
+      <c r="B8" s="36"/>
+      <c r="C8" s="36"/>
+      <c r="D8" s="36"/>
+      <c r="E8" s="36"/>
+      <c r="F8" s="36"/>
+      <c r="G8" s="36"/>
+      <c r="P8" s="38"/>
+    </row>
+    <row r="9" s="37" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="35"/>
+      <c r="B9" s="36"/>
+      <c r="C9" s="36"/>
+      <c r="D9" s="36"/>
+      <c r="E9" s="36"/>
+      <c r="F9" s="36"/>
+      <c r="G9" s="36"/>
+      <c r="P9" s="38" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="10" s="36" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="34"/>
-      <c r="B10" s="35"/>
-      <c r="C10" s="35"/>
-      <c r="D10" s="35"/>
-      <c r="E10" s="35"/>
-      <c r="F10" s="35"/>
-      <c r="G10" s="35"/>
-    </row>
-    <row r="11" s="36" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="34"/>
-      <c r="B11" s="35"/>
-      <c r="C11" s="35"/>
-      <c r="D11" s="35"/>
-      <c r="E11" s="35"/>
-      <c r="F11" s="35"/>
-      <c r="G11" s="35"/>
+    <row r="10" s="37" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="35"/>
+      <c r="B10" s="36"/>
+      <c r="C10" s="36"/>
+      <c r="D10" s="36"/>
+      <c r="E10" s="36"/>
+      <c r="F10" s="36"/>
+      <c r="G10" s="36"/>
+    </row>
+    <row r="11" s="37" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="35"/>
+      <c r="B11" s="36"/>
+      <c r="C11" s="36"/>
+      <c r="D11" s="36"/>
+      <c r="E11" s="36"/>
+      <c r="F11" s="36"/>
+      <c r="G11" s="36"/>
     </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="34"/>
-      <c r="B12" s="35"/>
-      <c r="C12" s="35"/>
-      <c r="D12" s="35"/>
-      <c r="E12" s="35"/>
-      <c r="F12" s="35"/>
-      <c r="G12" s="35"/>
+      <c r="A12" s="35"/>
+      <c r="B12" s="36"/>
+      <c r="C12" s="36"/>
+      <c r="D12" s="36"/>
+      <c r="E12" s="36"/>
+      <c r="F12" s="36"/>
+      <c r="G12" s="36"/>
     </row>
     <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="34"/>
-      <c r="B13" s="35"/>
-      <c r="C13" s="35"/>
-      <c r="D13" s="35"/>
-      <c r="E13" s="35"/>
-      <c r="F13" s="35"/>
-      <c r="G13" s="35"/>
+      <c r="A13" s="35"/>
+      <c r="B13" s="36"/>
+      <c r="C13" s="36"/>
+      <c r="D13" s="36"/>
+      <c r="E13" s="36"/>
+      <c r="F13" s="36"/>
+      <c r="G13" s="36"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -2644,19 +2847,19 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="F6" activeCellId="0" sqref="F6"/>
+      <selection pane="bottomLeft" activeCell="G7" activeCellId="0" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.77"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.79"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="45.77"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="50.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="50.79"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="45.77"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="11.77"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="40.78"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="8" style="0" width="14.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="8" style="0" width="14.43"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2669,7 +2872,7 @@
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
       <c r="G1" s="2"/>
-      <c r="P1" s="18"/>
+      <c r="P1" s="19"/>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="2"/>
@@ -2679,157 +2882,197 @@
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
-      <c r="P2" s="18"/>
-    </row>
-    <row r="3" s="32" customFormat="true" ht="28.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="29" t="s">
+      <c r="P2" s="19"/>
+    </row>
+    <row r="3" s="33" customFormat="true" ht="28.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="30" t="s">
+      <c r="B3" s="31" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="29" t="s">
+      <c r="C3" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="29" t="s">
+      <c r="D3" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="29" t="s">
+      <c r="E3" s="30" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="31" t="s">
+      <c r="F3" s="32" t="s">
         <v>6</v>
       </c>
-      <c r="G3" s="31" t="s">
+      <c r="G3" s="32" t="s">
         <v>7</v>
       </c>
-      <c r="P3" s="33"/>
-    </row>
-    <row r="4" s="36" customFormat="true" ht="125.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="34" t="s">
+      <c r="P3" s="34"/>
+    </row>
+    <row r="4" s="37" customFormat="true" ht="124.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="35" t="s">
         <v>95</v>
       </c>
-      <c r="B4" s="35" t="s">
+      <c r="B4" s="36" t="s">
         <v>96</v>
       </c>
-      <c r="C4" s="35" t="s">
+      <c r="C4" s="36" t="s">
         <v>97</v>
       </c>
-      <c r="D4" s="35" t="s">
+      <c r="D4" s="36" t="s">
         <v>98</v>
       </c>
-      <c r="E4" s="35" t="s">
+      <c r="E4" s="36" t="s">
         <v>99</v>
       </c>
-      <c r="F4" s="35" t="s">
+      <c r="F4" s="36" t="s">
         <v>13</v>
       </c>
-      <c r="G4" s="35" t="s">
+      <c r="G4" s="36" t="s">
         <v>100</v>
       </c>
-      <c r="O4" s="37" t="s">
+      <c r="O4" s="38" t="s">
         <v>68</v>
       </c>
-      <c r="P4" s="37" t="s">
+      <c r="P4" s="38" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="5" s="36" customFormat="true" ht="69" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="34" t="s">
+    <row r="5" s="37" customFormat="true" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="35" t="s">
         <v>101</v>
       </c>
-      <c r="B5" s="35" t="s">
+      <c r="B5" s="36" t="s">
         <v>96</v>
       </c>
-      <c r="C5" s="35" t="s">
+      <c r="C5" s="36" t="s">
         <v>102</v>
       </c>
-      <c r="D5" s="35" t="s">
+      <c r="D5" s="36" t="s">
         <v>103</v>
       </c>
-      <c r="E5" s="35" t="s">
+      <c r="E5" s="36" t="s">
         <v>104</v>
       </c>
-      <c r="F5" s="35" t="s">
+      <c r="F5" s="36" t="s">
         <v>13</v>
       </c>
-      <c r="G5" s="35" t="s">
+      <c r="G5" s="36" t="s">
         <v>105</v>
       </c>
-      <c r="P5" s="37" t="s">
+      <c r="P5" s="38" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="6" s="36" customFormat="true" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="34" t="s">
+    <row r="6" s="37" customFormat="true" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="35" t="s">
         <v>106</v>
       </c>
-      <c r="B6" s="35" t="s">
+      <c r="B6" s="36" t="s">
         <v>107</v>
       </c>
-      <c r="C6" s="35" t="s">
+      <c r="C6" s="36" t="s">
         <v>108</v>
       </c>
-      <c r="D6" s="35" t="s">
+      <c r="D6" s="36" t="s">
         <v>109</v>
       </c>
-      <c r="E6" s="35" t="s">
+      <c r="E6" s="36" t="s">
         <v>110</v>
       </c>
-      <c r="F6" s="35" t="s">
+      <c r="F6" s="36" t="s">
         <v>20</v>
       </c>
-      <c r="G6" s="35"/>
-      <c r="P6" s="37" t="s">
+      <c r="G6" s="36"/>
+      <c r="P6" s="38" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="7" s="36" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="34"/>
-      <c r="B7" s="35" t="s">
+    <row r="7" s="37" customFormat="true" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="35" t="s">
         <v>111</v>
       </c>
-      <c r="C7" s="35"/>
-      <c r="D7" s="35"/>
-      <c r="E7" s="35"/>
-      <c r="F7" s="35"/>
-      <c r="G7" s="35"/>
-    </row>
-    <row r="8" s="36" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="34"/>
-      <c r="B8" s="35"/>
-      <c r="C8" s="35"/>
-      <c r="D8" s="35"/>
-      <c r="E8" s="35"/>
-      <c r="F8" s="35"/>
-      <c r="G8" s="35"/>
-    </row>
-    <row r="9" s="36" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="34"/>
-      <c r="B9" s="35"/>
-      <c r="C9" s="35"/>
-      <c r="D9" s="35"/>
-      <c r="E9" s="35"/>
-      <c r="F9" s="35"/>
-      <c r="G9" s="35"/>
-    </row>
-    <row r="10" s="36" customFormat="true" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="34"/>
-      <c r="B10" s="35"/>
-      <c r="C10" s="35"/>
-      <c r="D10" s="35"/>
-      <c r="E10" s="35"/>
-      <c r="F10" s="35"/>
-      <c r="G10" s="35"/>
+      <c r="B7" s="36" t="s">
+        <v>112</v>
+      </c>
+      <c r="C7" s="36" t="s">
+        <v>113</v>
+      </c>
+      <c r="D7" s="36" t="s">
+        <v>114</v>
+      </c>
+      <c r="E7" s="36" t="s">
+        <v>115</v>
+      </c>
+      <c r="F7" s="36" t="s">
+        <v>13</v>
+      </c>
+      <c r="G7" s="36" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="8" s="37" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="35" t="s">
+        <v>117</v>
+      </c>
+      <c r="B8" s="40" t="s">
+        <v>96</v>
+      </c>
+      <c r="C8" s="36" t="s">
+        <v>118</v>
+      </c>
+      <c r="D8" s="41" t="s">
+        <v>119</v>
+      </c>
+      <c r="E8" s="36" t="s">
+        <v>120</v>
+      </c>
+      <c r="F8" s="36" t="s">
+        <v>13</v>
+      </c>
+      <c r="G8" s="36" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="9" s="37" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="35" t="s">
+        <v>121</v>
+      </c>
+      <c r="B9" s="40" t="s">
+        <v>96</v>
+      </c>
+      <c r="C9" s="36" t="s">
+        <v>122</v>
+      </c>
+      <c r="D9" s="41" t="s">
+        <v>123</v>
+      </c>
+      <c r="E9" s="36" t="s">
+        <v>124</v>
+      </c>
+      <c r="F9" s="36" t="s">
+        <v>13</v>
+      </c>
+      <c r="G9" s="36" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="10" s="37" customFormat="true" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A10" s="35"/>
+      <c r="B10" s="36"/>
+      <c r="C10" s="36"/>
+      <c r="D10" s="36"/>
+      <c r="E10" s="36"/>
+      <c r="F10" s="36"/>
+      <c r="G10" s="36"/>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="34"/>
-      <c r="B11" s="35"/>
-      <c r="C11" s="35"/>
-      <c r="D11" s="35"/>
-      <c r="E11" s="35"/>
-      <c r="F11" s="35"/>
-      <c r="G11" s="35"/>
+      <c r="A11" s="35"/>
+      <c r="B11" s="36"/>
+      <c r="C11" s="36"/>
+      <c r="D11" s="36"/>
+      <c r="E11" s="36"/>
+      <c r="F11" s="36"/>
+      <c r="G11" s="36"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -2862,15 +3105,15 @@
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F6" activeCellId="0" sqref="F6"/>
+      <selection pane="topLeft" activeCell="C6" activeCellId="0" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.77"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.79"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="45.77"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="50.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="50.79"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="45.77"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="11.77"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="40.78"/>
@@ -2879,7 +3122,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>112</v>
+        <v>126</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
@@ -2897,7 +3140,7 @@
       <c r="F2" s="2"/>
       <c r="G2" s="2"/>
     </row>
-    <row r="3" s="39" customFormat="true" ht="28.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="3" s="42" customFormat="true" ht="28.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
         <v>1</v>
       </c>
@@ -2905,7 +3148,7 @@
         <v>2</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>113</v>
+        <v>127</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>4</v>
@@ -2920,44 +3163,44 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="22" t="s">
-        <v>114</v>
-      </c>
-      <c r="B4" s="23" t="s">
-        <v>115</v>
-      </c>
-      <c r="C4" s="23" t="s">
-        <v>116</v>
-      </c>
-      <c r="D4" s="23" t="s">
-        <v>117</v>
-      </c>
-      <c r="E4" s="23" t="s">
-        <v>118</v>
+    <row r="4" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="23" t="s">
+        <v>128</v>
+      </c>
+      <c r="B4" s="24" t="s">
+        <v>129</v>
+      </c>
+      <c r="C4" s="24" t="s">
+        <v>130</v>
+      </c>
+      <c r="D4" s="24" t="s">
+        <v>131</v>
+      </c>
+      <c r="E4" s="24" t="s">
+        <v>132</v>
       </c>
       <c r="F4" s="10" t="s">
         <v>13</v>
       </c>
       <c r="G4" s="10" t="s">
-        <v>119</v>
+        <v>133</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="22" t="s">
-        <v>120</v>
-      </c>
-      <c r="B5" s="23" t="s">
-        <v>115</v>
-      </c>
-      <c r="C5" s="23" t="s">
-        <v>121</v>
-      </c>
-      <c r="D5" s="23" t="s">
-        <v>122</v>
-      </c>
-      <c r="E5" s="23" t="s">
-        <v>123</v>
+      <c r="A5" s="23" t="s">
+        <v>134</v>
+      </c>
+      <c r="B5" s="24" t="s">
+        <v>129</v>
+      </c>
+      <c r="C5" s="24" t="s">
+        <v>135</v>
+      </c>
+      <c r="D5" s="24" t="s">
+        <v>136</v>
+      </c>
+      <c r="E5" s="24" t="s">
+        <v>137</v>
       </c>
       <c r="F5" s="10" t="s">
         <v>20</v>
@@ -2965,45 +3208,61 @@
       <c r="G5" s="10"/>
     </row>
     <row r="6" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="22"/>
-      <c r="B6" s="23" t="s">
-        <v>124</v>
-      </c>
-      <c r="C6" s="23" t="s">
-        <v>125</v>
-      </c>
-      <c r="D6" s="23" t="s">
-        <v>126</v>
-      </c>
-      <c r="E6" s="23" t="s">
-        <v>127</v>
+      <c r="A6" s="23" t="s">
+        <v>138</v>
+      </c>
+      <c r="B6" s="24" t="s">
+        <v>139</v>
+      </c>
+      <c r="C6" s="24" t="s">
+        <v>140</v>
+      </c>
+      <c r="D6" s="24" t="s">
+        <v>141</v>
+      </c>
+      <c r="E6" s="24" t="s">
+        <v>142</v>
       </c>
       <c r="F6" s="10" t="s">
         <v>20</v>
       </c>
       <c r="G6" s="10"/>
     </row>
-    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="22"/>
-      <c r="B7" s="23"/>
-      <c r="C7" s="10"/>
-      <c r="D7" s="10"/>
-      <c r="E7" s="10"/>
-      <c r="F7" s="10"/>
-      <c r="G7" s="10"/>
+    <row r="7" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="23" t="s">
+        <v>143</v>
+      </c>
+      <c r="B7" s="43" t="s">
+        <v>139</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>144</v>
+      </c>
+      <c r="D7" s="11" t="s">
+        <v>145</v>
+      </c>
+      <c r="E7" s="11" t="s">
+        <v>146</v>
+      </c>
+      <c r="F7" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="G7" s="10" t="s">
+        <v>147</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="22"/>
-      <c r="B8" s="23"/>
+      <c r="A8" s="23"/>
+      <c r="B8" s="43"/>
       <c r="C8" s="10"/>
-      <c r="D8" s="10"/>
+      <c r="D8" s="11"/>
       <c r="E8" s="10"/>
       <c r="F8" s="10"/>
       <c r="G8" s="10"/>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="22"/>
-      <c r="B9" s="23"/>
+      <c r="A9" s="23"/>
+      <c r="B9" s="24"/>
       <c r="C9" s="10"/>
       <c r="D9" s="10"/>
       <c r="E9" s="10"/>
@@ -3011,8 +3270,8 @@
       <c r="G9" s="10"/>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="22"/>
-      <c r="B10" s="23"/>
+      <c r="A10" s="23"/>
+      <c r="B10" s="24"/>
       <c r="C10" s="10"/>
       <c r="D10" s="10"/>
       <c r="E10" s="10"/>
@@ -3020,8 +3279,8 @@
       <c r="G10" s="10"/>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="22"/>
-      <c r="B11" s="23"/>
+      <c r="A11" s="23"/>
+      <c r="B11" s="24"/>
       <c r="C11" s="10"/>
       <c r="D11" s="10"/>
       <c r="E11" s="10"/>
@@ -3057,228 +3316,228 @@
     <tabColor rgb="FFFF0000"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I15"/>
+  <dimension ref="A1:I16"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H13" activeCellId="0" sqref="H13"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B18" activeCellId="0" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="40" width="6.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="40" width="8.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="40" width="9.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="40" width="10.22"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="40" width="32.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="6" style="40" width="35.44"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="40" width="35"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="40" width="33.22"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="10" style="40" width="8.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="44" width="6.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="44" width="8.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="44" width="9.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="44" width="10.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="44" width="32.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="6" style="44" width="35.44"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="44" width="35"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="44" width="33.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="10" style="44" width="8.89"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="28.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="41" t="s">
-        <v>128</v>
-      </c>
-      <c r="B1" s="41"/>
-      <c r="C1" s="41"/>
-      <c r="D1" s="41"/>
-      <c r="E1" s="41"/>
-      <c r="F1" s="41"/>
-      <c r="G1" s="41"/>
-      <c r="H1" s="41"/>
-      <c r="I1" s="41"/>
+      <c r="A1" s="45" t="s">
+        <v>148</v>
+      </c>
+      <c r="B1" s="45"/>
+      <c r="C1" s="45"/>
+      <c r="D1" s="45"/>
+      <c r="E1" s="45"/>
+      <c r="F1" s="45"/>
+      <c r="G1" s="45"/>
+      <c r="H1" s="45"/>
+      <c r="I1" s="45"/>
     </row>
     <row r="2" customFormat="false" ht="21" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="41"/>
-      <c r="B2" s="41"/>
-      <c r="C2" s="41"/>
-      <c r="D2" s="41"/>
-      <c r="E2" s="41"/>
-      <c r="F2" s="41"/>
-      <c r="G2" s="41"/>
-      <c r="H2" s="41"/>
-      <c r="I2" s="41"/>
-    </row>
-    <row r="3" s="46" customFormat="true" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="42" t="s">
-        <v>129</v>
-      </c>
-      <c r="B3" s="43" t="s">
+      <c r="A2" s="45"/>
+      <c r="B2" s="45"/>
+      <c r="C2" s="45"/>
+      <c r="D2" s="45"/>
+      <c r="E2" s="45"/>
+      <c r="F2" s="45"/>
+      <c r="G2" s="45"/>
+      <c r="H2" s="45"/>
+      <c r="I2" s="45"/>
+    </row>
+    <row r="3" s="50" customFormat="true" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="46" t="s">
+        <v>149</v>
+      </c>
+      <c r="B3" s="47" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="43" t="s">
-        <v>130</v>
-      </c>
-      <c r="D3" s="43" t="s">
-        <v>131</v>
-      </c>
-      <c r="E3" s="43" t="s">
-        <v>132</v>
-      </c>
-      <c r="F3" s="43" t="s">
-        <v>133</v>
-      </c>
-      <c r="G3" s="43" t="s">
-        <v>134</v>
-      </c>
-      <c r="H3" s="44" t="s">
-        <v>135</v>
-      </c>
-      <c r="I3" s="45" t="s">
+      <c r="C3" s="47" t="s">
+        <v>150</v>
+      </c>
+      <c r="D3" s="47" t="s">
+        <v>151</v>
+      </c>
+      <c r="E3" s="47" t="s">
+        <v>152</v>
+      </c>
+      <c r="F3" s="47" t="s">
+        <v>153</v>
+      </c>
+      <c r="G3" s="47" t="s">
+        <v>154</v>
+      </c>
+      <c r="H3" s="48" t="s">
+        <v>155</v>
+      </c>
+      <c r="I3" s="49" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="47" t="n">
+      <c r="A4" s="51" t="n">
         <v>1</v>
       </c>
       <c r="B4" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="15" t="s">
-        <v>136</v>
+      <c r="C4" s="16" t="s">
+        <v>156</v>
       </c>
       <c r="D4" s="10" t="s">
-        <v>137</v>
+        <v>157</v>
       </c>
       <c r="E4" s="10" t="s">
-        <v>138</v>
-      </c>
-      <c r="F4" s="48" t="s">
-        <v>139</v>
-      </c>
-      <c r="G4" s="15" t="s">
-        <v>140</v>
-      </c>
-      <c r="H4" s="15" t="s">
-        <v>141</v>
+        <v>158</v>
+      </c>
+      <c r="F4" s="52" t="s">
+        <v>159</v>
+      </c>
+      <c r="G4" s="16" t="s">
+        <v>160</v>
+      </c>
+      <c r="H4" s="16" t="s">
+        <v>161</v>
       </c>
       <c r="I4" s="10"/>
     </row>
     <row r="5" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="47" t="n">
+      <c r="A5" s="51" t="n">
         <v>2</v>
       </c>
       <c r="B5" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="C5" s="15" t="s">
-        <v>142</v>
+      <c r="C5" s="16" t="s">
+        <v>162</v>
       </c>
       <c r="D5" s="10" t="s">
-        <v>142</v>
-      </c>
-      <c r="E5" s="15" t="s">
-        <v>143</v>
-      </c>
-      <c r="F5" s="48" t="s">
-        <v>144</v>
-      </c>
-      <c r="G5" s="15" t="s">
+        <v>162</v>
+      </c>
+      <c r="E5" s="16" t="s">
+        <v>163</v>
+      </c>
+      <c r="F5" s="52" t="s">
+        <v>164</v>
+      </c>
+      <c r="G5" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="H5" s="15" t="s">
-        <v>145</v>
-      </c>
-      <c r="I5" s="15"/>
-    </row>
-    <row r="6" customFormat="false" ht="113.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="47" t="n">
+      <c r="H5" s="16" t="s">
+        <v>165</v>
+      </c>
+      <c r="I5" s="16"/>
+    </row>
+    <row r="6" customFormat="false" ht="114" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="51" t="n">
         <v>3</v>
       </c>
-      <c r="B6" s="49" t="s">
+      <c r="B6" s="53" t="s">
         <v>32</v>
       </c>
-      <c r="C6" s="15" t="s">
-        <v>142</v>
+      <c r="C6" s="16" t="s">
+        <v>162</v>
       </c>
       <c r="D6" s="10" t="s">
-        <v>142</v>
+        <v>162</v>
       </c>
       <c r="E6" s="10" t="s">
-        <v>146</v>
-      </c>
-      <c r="F6" s="48" t="s">
+        <v>166</v>
+      </c>
+      <c r="F6" s="52" t="s">
         <v>34</v>
       </c>
-      <c r="G6" s="48" t="s">
-        <v>147</v>
+      <c r="G6" s="52" t="s">
+        <v>167</v>
       </c>
       <c r="H6" s="10" t="s">
-        <v>148</v>
+        <v>168</v>
       </c>
       <c r="I6" s="10"/>
     </row>
     <row r="7" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="47" t="n">
+      <c r="A7" s="51" t="n">
         <v>4</v>
       </c>
-      <c r="B7" s="49" t="s">
+      <c r="B7" s="53" t="s">
         <v>52</v>
       </c>
-      <c r="C7" s="15" t="s">
-        <v>149</v>
+      <c r="C7" s="16" t="s">
+        <v>169</v>
       </c>
       <c r="D7" s="10" t="s">
-        <v>136</v>
+        <v>156</v>
       </c>
       <c r="E7" s="10" t="s">
-        <v>150</v>
-      </c>
-      <c r="F7" s="48" t="s">
+        <v>170</v>
+      </c>
+      <c r="F7" s="52" t="s">
         <v>54</v>
       </c>
-      <c r="G7" s="48" t="s">
+      <c r="G7" s="52" t="s">
         <v>55</v>
       </c>
       <c r="H7" s="10" t="s">
-        <v>151</v>
+        <v>171</v>
       </c>
       <c r="I7" s="10"/>
     </row>
     <row r="8" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="47" t="n">
+      <c r="A8" s="51" t="n">
         <v>5</v>
       </c>
-      <c r="B8" s="50" t="s">
+      <c r="B8" s="54" t="s">
         <v>62</v>
       </c>
-      <c r="C8" s="15" t="s">
-        <v>136</v>
+      <c r="C8" s="16" t="s">
+        <v>156</v>
       </c>
       <c r="D8" s="10" t="s">
-        <v>142</v>
+        <v>162</v>
       </c>
       <c r="E8" s="10" t="s">
-        <v>152</v>
+        <v>172</v>
       </c>
       <c r="F8" s="10" t="s">
-        <v>153</v>
+        <v>173</v>
       </c>
       <c r="G8" s="10" t="s">
-        <v>154</v>
+        <v>174</v>
       </c>
       <c r="H8" s="10" t="s">
-        <v>155</v>
+        <v>175</v>
       </c>
       <c r="I8" s="10"/>
     </row>
     <row r="9" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="47" t="n">
+      <c r="A9" s="51" t="n">
         <v>6</v>
       </c>
-      <c r="B9" s="50" t="s">
+      <c r="B9" s="54" t="s">
         <v>70</v>
       </c>
-      <c r="C9" s="15" t="s">
-        <v>149</v>
+      <c r="C9" s="16" t="s">
+        <v>169</v>
       </c>
       <c r="D9" s="10" t="s">
-        <v>136</v>
+        <v>156</v>
       </c>
       <c r="E9" s="10" t="s">
-        <v>156</v>
+        <v>176</v>
       </c>
       <c r="F9" s="10" t="s">
         <v>72</v>
@@ -3287,144 +3546,209 @@
         <v>44</v>
       </c>
       <c r="H9" s="10" t="s">
-        <v>157</v>
+        <v>177</v>
       </c>
       <c r="I9" s="10"/>
     </row>
     <row r="10" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="47" t="n">
+      <c r="A10" s="51" t="n">
         <v>7</v>
       </c>
-      <c r="B10" s="51" t="s">
+      <c r="B10" s="55" t="s">
         <v>75</v>
       </c>
-      <c r="C10" s="15" t="s">
-        <v>142</v>
+      <c r="C10" s="16" t="s">
+        <v>162</v>
       </c>
       <c r="D10" s="10" t="s">
-        <v>158</v>
+        <v>178</v>
       </c>
       <c r="E10" s="10" t="s">
-        <v>159</v>
-      </c>
-      <c r="F10" s="48" t="s">
+        <v>179</v>
+      </c>
+      <c r="F10" s="52" t="s">
         <v>77</v>
       </c>
-      <c r="G10" s="48" t="s">
+      <c r="G10" s="52" t="s">
         <v>78</v>
       </c>
       <c r="H10" s="10" t="s">
-        <v>160</v>
+        <v>180</v>
       </c>
       <c r="I10" s="10"/>
     </row>
     <row r="11" customFormat="false" ht="147" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="47" t="n">
+      <c r="A11" s="51" t="n">
         <v>8</v>
       </c>
-      <c r="B11" s="51"/>
-      <c r="C11" s="15" t="s">
-        <v>136</v>
+      <c r="B11" s="55" t="s">
+        <v>95</v>
+      </c>
+      <c r="C11" s="16" t="s">
+        <v>156</v>
       </c>
       <c r="D11" s="10" t="s">
-        <v>136</v>
+        <v>156</v>
       </c>
       <c r="E11" s="10" t="s">
-        <v>161</v>
+        <v>181</v>
       </c>
       <c r="F11" s="10" t="s">
+        <v>182</v>
+      </c>
+      <c r="G11" s="10" t="s">
+        <v>183</v>
+      </c>
+      <c r="H11" s="10" t="s">
+        <v>184</v>
+      </c>
+      <c r="I11" s="10"/>
+    </row>
+    <row r="12" customFormat="false" ht="80.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="51" t="n">
+        <v>9</v>
+      </c>
+      <c r="B12" s="55" t="s">
+        <v>117</v>
+      </c>
+      <c r="C12" s="16" t="s">
         <v>162</v>
       </c>
-      <c r="G11" s="10" t="s">
-        <v>163</v>
-      </c>
-      <c r="H11" s="10" t="s">
-        <v>164</v>
-      </c>
-      <c r="I11" s="10"/>
-    </row>
-    <row r="12" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="47" t="n">
-        <v>9</v>
-      </c>
-      <c r="B12" s="51"/>
-      <c r="C12" s="15" t="s">
-        <v>142</v>
-      </c>
       <c r="D12" s="10" t="s">
-        <v>158</v>
+        <v>185</v>
       </c>
       <c r="E12" s="10" t="s">
-        <v>165</v>
+        <v>186</v>
       </c>
       <c r="F12" s="10" t="s">
-        <v>166</v>
+        <v>187</v>
       </c>
       <c r="G12" s="10" t="s">
-        <v>167</v>
+        <v>188</v>
       </c>
       <c r="H12" s="10" t="s">
-        <v>168</v>
+        <v>189</v>
       </c>
       <c r="I12" s="10"/>
     </row>
     <row r="13" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="47" t="n">
+      <c r="A13" s="51" t="n">
         <v>10</v>
       </c>
-      <c r="B13" s="51"/>
-      <c r="C13" s="15" t="s">
-        <v>136</v>
+      <c r="B13" s="55" t="s">
+        <v>128</v>
+      </c>
+      <c r="C13" s="16" t="s">
+        <v>156</v>
       </c>
       <c r="D13" s="10" t="s">
-        <v>136</v>
-      </c>
-      <c r="E13" s="52" t="s">
+        <v>156</v>
+      </c>
+      <c r="E13" s="56" t="s">
+        <v>190</v>
+      </c>
+      <c r="F13" s="57" t="s">
+        <v>191</v>
+      </c>
+      <c r="G13" s="57" t="s">
+        <v>192</v>
+      </c>
+      <c r="H13" s="56" t="s">
+        <v>193</v>
+      </c>
+      <c r="I13" s="57"/>
+    </row>
+    <row r="14" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="51" t="n">
+        <v>11</v>
+      </c>
+      <c r="B14" s="55" t="s">
+        <v>143</v>
+      </c>
+      <c r="C14" s="16" t="s">
+        <v>156</v>
+      </c>
+      <c r="D14" s="10" t="s">
         <v>169</v>
       </c>
-      <c r="F13" s="53" t="s">
-        <v>170</v>
-      </c>
-      <c r="G13" s="53" t="s">
-        <v>171</v>
-      </c>
-      <c r="H13" s="52" t="s">
-        <v>172</v>
-      </c>
-      <c r="I13" s="53"/>
-    </row>
-    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="47"/>
-      <c r="B14" s="51"/>
-      <c r="C14" s="15"/>
-      <c r="D14" s="10"/>
-      <c r="E14" s="52"/>
-      <c r="F14" s="53"/>
-      <c r="G14" s="53"/>
-      <c r="H14" s="52"/>
-      <c r="I14" s="53"/>
-    </row>
-    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="47"/>
-      <c r="B15" s="51"/>
-      <c r="C15" s="15"/>
-      <c r="D15" s="10"/>
-      <c r="E15" s="52"/>
-      <c r="F15" s="53"/>
-      <c r="G15" s="53"/>
-      <c r="H15" s="52"/>
-      <c r="I15" s="53"/>
+      <c r="E14" s="56" t="s">
+        <v>194</v>
+      </c>
+      <c r="F14" s="11" t="s">
+        <v>145</v>
+      </c>
+      <c r="G14" s="11" t="s">
+        <v>195</v>
+      </c>
+      <c r="H14" s="56" t="s">
+        <v>196</v>
+      </c>
+      <c r="I14" s="57"/>
+    </row>
+    <row r="15" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="51" t="n">
+        <v>12</v>
+      </c>
+      <c r="B15" s="55" t="s">
+        <v>121</v>
+      </c>
+      <c r="C15" s="16" t="s">
+        <v>162</v>
+      </c>
+      <c r="D15" s="10" t="s">
+        <v>178</v>
+      </c>
+      <c r="E15" s="56" t="s">
+        <v>197</v>
+      </c>
+      <c r="F15" s="11" t="s">
+        <v>123</v>
+      </c>
+      <c r="G15" s="11" t="s">
+        <v>124</v>
+      </c>
+      <c r="H15" s="56" t="s">
+        <v>198</v>
+      </c>
+      <c r="I15" s="57"/>
+    </row>
+    <row r="16" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="51" t="n">
+        <v>13</v>
+      </c>
+      <c r="B16" s="55" t="s">
+        <v>111</v>
+      </c>
+      <c r="C16" s="16" t="s">
+        <v>162</v>
+      </c>
+      <c r="D16" s="10" t="s">
+        <v>162</v>
+      </c>
+      <c r="E16" s="56" t="s">
+        <v>199</v>
+      </c>
+      <c r="F16" s="11" t="s">
+        <v>200</v>
+      </c>
+      <c r="G16" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="H16" s="56" t="s">
+        <v>180</v>
+      </c>
+      <c r="I16" s="57"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:I2"/>
   </mergeCells>
   <dataValidations count="2">
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="C4:C15" type="list">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="C4:C16" type="list">
       <formula1>"High,Medium,Low,Not Planned"</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="D4:D15" type="list">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="true" sqref="D4:D16" type="list">
       <formula1>"Blocking,Critical,High,Medium,Low"</formula1>
       <formula2>0</formula2>
     </dataValidation>

</xml_diff>